<commit_message>
improve the main.py to make sure it loops through and will logger all model types listed
</commit_message>
<xml_diff>
--- a/AI_Challenges/week07/results.xlsx
+++ b/AI_Challenges/week07/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,7 +486,55 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>0.8824020016680567</v>
+        <v>0.8874061718098415</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>gated_cnn</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="C3" t="n">
+        <v>128</v>
+      </c>
+      <c r="D3" t="n">
+        <v>64</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>0.8807339449541285</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>gated_cnn</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="C4" t="n">
+        <v>128</v>
+      </c>
+      <c r="D4" t="n">
+        <v>256</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>avg</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>0.8840700583819849</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modify the readme files to make it clear
</commit_message>
<xml_diff>
--- a/AI_Challenges/week07/results.xlsx
+++ b/AI_Challenges/week07/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,7 +486,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>0.8874061718098415</v>
+        <v>0.8744787322768974</v>
       </c>
     </row>
     <row r="3">
@@ -510,7 +510,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>0.8807339449541285</v>
+        <v>0.8836530442035029</v>
       </c>
     </row>
     <row r="4">
@@ -534,7 +534,271 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>0.8840700583819849</v>
+        <v>0.8949124270225187</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>gated_cnn</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="C5" t="n">
+        <v>128</v>
+      </c>
+      <c r="D5" t="n">
+        <v>256</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>0.8878231859883235</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>gated_cnn</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="C6" t="n">
+        <v>256</v>
+      </c>
+      <c r="D6" t="n">
+        <v>64</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>avg</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>0.8669724770642202</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>gated_cnn</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="C7" t="n">
+        <v>256</v>
+      </c>
+      <c r="D7" t="n">
+        <v>64</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>0.8811509591326105</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>gated_cnn</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="C8" t="n">
+        <v>256</v>
+      </c>
+      <c r="D8" t="n">
+        <v>256</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>avg</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>0.8811509591326105</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>gated_cnn</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="C9" t="n">
+        <v>256</v>
+      </c>
+      <c r="D9" t="n">
+        <v>256</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>0.8886572143452878</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>gated_cnn</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="C10" t="n">
+        <v>128</v>
+      </c>
+      <c r="D10" t="n">
+        <v>64</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>avg</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>0.8786488740617181</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>gated_cnn</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="C11" t="n">
+        <v>128</v>
+      </c>
+      <c r="D11" t="n">
+        <v>64</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>0.8928273561301084</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>gated_cnn</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="C12" t="n">
+        <v>128</v>
+      </c>
+      <c r="D12" t="n">
+        <v>256</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>avg</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>0.8432026688907422</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>gated_cnn</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="C13" t="n">
+        <v>128</v>
+      </c>
+      <c r="D13" t="n">
+        <v>256</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>0.872393661384487</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>fast_text</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="C14" t="n">
+        <v>128</v>
+      </c>
+      <c r="D14" t="n">
+        <v>64</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>avg</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>0.8915763135946623</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>lstm</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="C15" t="n">
+        <v>128</v>
+      </c>
+      <c r="D15" t="n">
+        <v>64</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>avg</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>0.8798999165971643</v>
       </c>
     </row>
   </sheetData>

</xml_diff>